<commit_message>
-plumbing infpu field halfway done
- input field now reciving data can create inputs based on that
-it can catch input id and price

-have to build out submit method
-before that have to create pages complectely with daisy and tailwind
</commit_message>
<xml_diff>
--- a/backend/data/contracts/contractData/all_info.xlsx
+++ b/backend/data/contracts/contractData/all_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\projects\MY_PROJECTS\web_application\backend\data\contracts\contractData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82D9CEE-FB6D-40A0-9163-C649926184CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BF7CC4-1047-49B0-BC0B-DB2559B37605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7695" yWindow="4560" windowWidth="14745" windowHeight="7815" activeTab="1" xr2:uid="{4AAAB276-E881-4B9F-B447-DB4F3993933A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{4AAAB276-E881-4B9F-B447-DB4F3993933A}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Project Stages" sheetId="1" r:id="rId3"/>
     <sheet name="SLS 573 Elements" sheetId="4" r:id="rId4"/>
     <sheet name="Sub Contract works" sheetId="5" r:id="rId5"/>
+    <sheet name="material" sheetId="7" r:id="rId6"/>
+    <sheet name="material on brand" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="100">
   <si>
     <t>Preliminaries</t>
   </si>
@@ -330,6 +332,36 @@
   </si>
   <si>
     <t>Sub Structure</t>
+  </si>
+  <si>
+    <t>plumbing</t>
+  </si>
+  <si>
+    <t>electrical</t>
+  </si>
+  <si>
+    <t>wall finishes</t>
+  </si>
+  <si>
+    <t>floor &amp; wall tiles</t>
+  </si>
+  <si>
+    <t>cement</t>
+  </si>
+  <si>
+    <t>steel</t>
+  </si>
+  <si>
+    <t>sand</t>
+  </si>
+  <si>
+    <t>brick</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>plumStandardId</t>
   </si>
 </sst>
 </file>
@@ -383,7 +415,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -397,6 +429,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -903,7 +938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F9FA20A-B232-4B37-B2C6-2EBD34237702}">
   <dimension ref="A2:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -965,15 +1000,15 @@
         <v>"Bandara`s Company"</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f>_xlfn.CONCAT(""""&amp;B3&amp;"""")</f>
+        <f t="shared" ref="E3:F9" si="1">_xlfn.CONCAT(""""&amp;B3&amp;"""")</f>
         <v>"Bandara"</v>
       </c>
       <c r="F3" s="3" t="str">
-        <f>_xlfn.CONCAT(""""&amp;C3&amp;"""")</f>
+        <f t="shared" si="1"/>
         <v>"Rathnayake"</v>
       </c>
       <c r="G3" s="4" t="str">
-        <f t="shared" ref="G3:G9" si="1">_xlfn.CONCAT( "(",A3,", ", B3,", ", C3,")")</f>
+        <f t="shared" ref="G3:G9" si="2">_xlfn.CONCAT( "(",A3,", ", B3,", ", C3,")")</f>
         <v>(Bandara`s Company, Bandara, Rathnayake)</v>
       </c>
     </row>
@@ -992,15 +1027,15 @@
         <v>"Premasiri`s Company"</v>
       </c>
       <c r="E4" s="3" t="str">
-        <f>_xlfn.CONCAT(""""&amp;B4&amp;"""")</f>
+        <f t="shared" si="1"/>
         <v>" Premasiri"</v>
       </c>
       <c r="F4" s="3" t="str">
-        <f>_xlfn.CONCAT(""""&amp;C4&amp;"""")</f>
+        <f t="shared" si="1"/>
         <v>"Fenando"</v>
       </c>
       <c r="G4" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Premasiri`s Company,  Premasiri, Fenando)</v>
       </c>
     </row>
@@ -1019,15 +1054,15 @@
         <v>"Susantha`s Company"</v>
       </c>
       <c r="E5" s="3" t="str">
-        <f>_xlfn.CONCAT(""""&amp;B5&amp;"""")</f>
+        <f t="shared" si="1"/>
         <v>"Susantha"</v>
       </c>
       <c r="F5" s="3" t="str">
-        <f>_xlfn.CONCAT(""""&amp;C5&amp;"""")</f>
+        <f t="shared" si="1"/>
         <v>"Weerasinghe"</v>
       </c>
       <c r="G5" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Susantha`s Company, Susantha, Weerasinghe)</v>
       </c>
     </row>
@@ -1046,15 +1081,15 @@
         <v>"Niml`s Company"</v>
       </c>
       <c r="E6" s="3" t="str">
-        <f>_xlfn.CONCAT(""""&amp;B6&amp;"""")</f>
+        <f t="shared" si="1"/>
         <v>"Nimal"</v>
       </c>
       <c r="F6" s="3" t="str">
-        <f>_xlfn.CONCAT(""""&amp;C6&amp;"""")</f>
+        <f t="shared" si="1"/>
         <v>"Rathnayake"</v>
       </c>
       <c r="G6" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Niml`s Company, Nimal, Rathnayake)</v>
       </c>
     </row>
@@ -1073,15 +1108,15 @@
         <v>"Pradeep`s Company"</v>
       </c>
       <c r="E7" s="3" t="str">
-        <f>_xlfn.CONCAT(""""&amp;B7&amp;"""")</f>
+        <f t="shared" si="1"/>
         <v>"Pradeep"</v>
       </c>
       <c r="F7" s="3" t="str">
-        <f>_xlfn.CONCAT(""""&amp;C7&amp;"""")</f>
+        <f t="shared" si="1"/>
         <v>"Niroshan"</v>
       </c>
       <c r="G7" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Pradeep`s Company, Pradeep, Niroshan)</v>
       </c>
     </row>
@@ -1100,15 +1135,15 @@
         <v>"Buddhika`s Company"</v>
       </c>
       <c r="E8" s="3" t="str">
-        <f>_xlfn.CONCAT(""""&amp;B8&amp;"""")</f>
+        <f t="shared" si="1"/>
         <v>"Buddhika"</v>
       </c>
       <c r="F8" s="3" t="str">
-        <f>_xlfn.CONCAT(""""&amp;C8&amp;"""")</f>
+        <f t="shared" si="1"/>
         <v>"Nawarunna"</v>
       </c>
       <c r="G8" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Buddhika`s Company, Buddhika, Nawarunna)</v>
       </c>
     </row>
@@ -1127,15 +1162,15 @@
         <v>"Keerthi`s Company"</v>
       </c>
       <c r="E9" s="3" t="str">
-        <f>_xlfn.CONCAT(""""&amp;B9&amp;"""")</f>
+        <f t="shared" si="1"/>
         <v>"Keerthi"</v>
       </c>
       <c r="F9" s="3" t="str">
-        <f>_xlfn.CONCAT(""""&amp;C9&amp;"""")</f>
+        <f t="shared" si="1"/>
         <v>"Welagedara"</v>
       </c>
       <c r="G9" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>(Keerthi`s Company, Keerthi, Welagedara)</v>
       </c>
     </row>
@@ -1149,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37441751-FEB9-4E1F-9733-8A925E8D0EF3}">
   <dimension ref="A2:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1701,4 +1736,273 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968B0CA3-578D-4C2D-A708-9F641FDCCE05}">
+  <dimension ref="A2:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <f>_xlfn.CONCAT(""""&amp;A2&amp;"""")</f>
+        <v>"plumbing"</v>
+      </c>
+      <c r="C2" s="2" t="str">
+        <f>_xlfn.CONCAT( "(",B2,")")</f>
+        <v>("plumbing")</v>
+      </c>
+      <c r="D2" t="str" cm="1">
+        <f t="array" ref="D2">_xlfn.CONCAT("INSERT INTO material (material) VALUES",(TRANSPOSE(C2:C9)&amp;","))</f>
+        <v>INSERT INTO material (material) VALUES("plumbing"),("wall finishes"),("floor &amp; wall tiles"),("cement"),("sand"),("steel"),("brick"),("electrical"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f t="shared" ref="B3:B14" si="0">_xlfn.CONCAT(""""&amp;A3&amp;"""")</f>
+        <v>"wall finishes"</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <f t="shared" ref="C3:C14" si="1">_xlfn.CONCAT( "(",B3,")")</f>
+        <v>("wall finishes")</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>"floor &amp; wall tiles"</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>("floor &amp; wall tiles")</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>"cement"</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>("cement")</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>"sand"</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>("sand")</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>"steel"</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>("steel")</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>"brick"</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>("brick")</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>"electrical"</v>
+      </c>
+      <c r="C9" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>("electrical")</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76B38A99-EAFE-487D-ABD2-B48945462E41}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="74.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f>_xlfn.CONCAT( "(",A2,", ", B2,")")</f>
+        <v>(1, 1)</v>
+      </c>
+      <c r="D2" s="5" t="str" cm="1">
+        <f t="array" ref="D2">_xlfn.CONCAT("INSERT INTO brands_on_materials (material_id,brand_id) VALUES",(TRANSPOSE(C2:C4)&amp;","))</f>
+        <v>INSERT INTO brands_on_materials (material_id,brand_id) VALUES(1, 1),(1, 2),(1, 3),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f t="shared" ref="C3:C14" si="0">_xlfn.CONCAT( "(",A3,", ", B3,")")</f>
+        <v>(1, 2)</v>
+      </c>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>(1, 3)</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>